<commit_message>
analyzing and editing report
</commit_message>
<xml_diff>
--- a/tempfiles/graphs.xlsx
+++ b/tempfiles/graphs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="23">
   <si>
     <t>BFS</t>
   </si>
@@ -83,12 +83,18 @@
   <si>
     <t>Kernel 3</t>
   </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +134,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -152,7 +162,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -206,8 +216,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -220,8 +238,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -248,6 +270,10 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -274,6 +300,10 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,11 +576,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2133809288"/>
-        <c:axId val="-2133807016"/>
+        <c:axId val="-2138046280"/>
+        <c:axId val="2129198968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133809288"/>
+        <c:axId val="-2138046280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +589,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133807016"/>
+        <c:crossAx val="2129198968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -567,7 +597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133807016"/>
+        <c:axId val="2129198968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600.0"/>
@@ -598,7 +628,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133809288"/>
+        <c:crossAx val="-2138046280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -892,11 +922,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2116919768"/>
-        <c:axId val="-2076908584"/>
+        <c:axId val="-2134750680"/>
+        <c:axId val="-2134747736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2116919768"/>
+        <c:axId val="-2134750680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -905,7 +935,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2076908584"/>
+        <c:crossAx val="-2134747736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -913,7 +943,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2076908584"/>
+        <c:axId val="-2134747736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -943,7 +973,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116919768"/>
+        <c:crossAx val="-2134750680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,11 +1489,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2133813560"/>
-        <c:axId val="-2073100104"/>
+        <c:axId val="-2134699976"/>
+        <c:axId val="-2134696920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2133813560"/>
+        <c:axId val="-2134699976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1472,7 +1502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073100104"/>
+        <c:crossAx val="-2134696920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1480,7 +1510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2073100104"/>
+        <c:axId val="-2134696920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1491,7 +1521,687 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133813560"/>
+        <c:crossAx val="-2134699976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Temperature (C)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GTX 650</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Btree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PathFinder</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LUD</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Gaussian</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hotspot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$85:$D$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.458333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>36.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Quadro M6000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Btree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PathFinder</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LUD</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Gaussian</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hotspot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$85:$E$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.78505699999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>GTX 630</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$85:$F$91</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37.538462</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40.886267</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>36.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2107345304"/>
+        <c:axId val="-2107342360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2107345304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107342360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2107342360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Celsius</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107345304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400"/>
+              <a:t>Fan (%)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>GTX 650</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Btree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PathFinder</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LUD</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Gaussian</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hotspot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$108:$D$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Quadro M6000</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>BFS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>NN</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Btree</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>PathFinder</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>LUD</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Gaussian</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Hotspot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$108:$E$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.032502</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>GTX 630</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$108:$F$114</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2106388856"/>
+        <c:axId val="-2106385880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2106388856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2106385880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2106385880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>%</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2106388856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1609,6 +2319,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1939,10 +2713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F72"/>
+  <dimension ref="A2:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2461,6 +3235,230 @@
       </c>
       <c r="F72" s="7">
         <v>36</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="C85" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="E85" s="1">
+        <v>77</v>
+      </c>
+      <c r="F85" s="8">
+        <v>37.538462000000003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="1">
+        <v>36</v>
+      </c>
+      <c r="E86" s="1">
+        <v>72</v>
+      </c>
+      <c r="F86" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="C87" t="s">
+        <v>2</v>
+      </c>
+      <c r="D87" s="1">
+        <v>36.458333000000003</v>
+      </c>
+      <c r="E87" s="1">
+        <v>76</v>
+      </c>
+      <c r="F87" s="8">
+        <v>36.840000000000003</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="C88" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" s="1">
+        <v>21</v>
+      </c>
+      <c r="E88" s="1">
+        <v>82.785056999999995</v>
+      </c>
+      <c r="F88" s="8">
+        <v>40.886266999999997</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" s="1">
+        <v>36</v>
+      </c>
+      <c r="E89" s="1">
+        <v>74</v>
+      </c>
+      <c r="F89" s="8">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="C90" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="1">
+        <v>37</v>
+      </c>
+      <c r="E90" s="1">
+        <v>77</v>
+      </c>
+      <c r="F90" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+      <c r="D91" s="1">
+        <v>36.75</v>
+      </c>
+      <c r="E91" s="1">
+        <v>74</v>
+      </c>
+      <c r="F91" s="8">
+        <v>38.1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" t="s">
+        <v>22</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
+      </c>
+      <c r="E107" t="s">
+        <v>8</v>
+      </c>
+      <c r="F107" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="C108" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="1">
+        <v>21</v>
+      </c>
+      <c r="E108" s="1">
+        <v>30</v>
+      </c>
+      <c r="F108" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="C109" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" s="1">
+        <v>21</v>
+      </c>
+      <c r="E109" s="1">
+        <v>30</v>
+      </c>
+      <c r="F109" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="C110" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="1">
+        <v>21</v>
+      </c>
+      <c r="E110" s="1">
+        <v>30</v>
+      </c>
+      <c r="F110" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="C111" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="1">
+        <v>21</v>
+      </c>
+      <c r="E111" s="1">
+        <v>35.032502000000001</v>
+      </c>
+      <c r="F111" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112" s="1">
+        <v>21</v>
+      </c>
+      <c r="E112" s="1">
+        <v>30</v>
+      </c>
+      <c r="F112" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" spans="3:6">
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+      <c r="D113" s="1">
+        <v>21</v>
+      </c>
+      <c r="E113" s="1">
+        <v>30</v>
+      </c>
+      <c r="F113" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="114" spans="3:6">
+      <c r="C114" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="1">
+        <v>21</v>
+      </c>
+      <c r="E114" s="1">
+        <v>30</v>
+      </c>
+      <c r="F114" s="8">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>